<commit_message>
Thêm các FK còn thiếu, xóa cột staff_id của schedule, insert data & thêm file template
</commit_message>
<xml_diff>
--- a/Database/data java2/Permission.xlsx
+++ b/Database/data java2/Permission.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\data java2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vuduc\Desktop\Project2\Database\data java2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0C798486-6D89-4370-8403-E2A4E753E7B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25EA42CE-8979-4ABC-9991-48E00EA5EB6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{41566BB7-1865-45BC-91BF-7FDFC46EBD65}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{41566BB7-1865-45BC-91BF-7FDFC46EBD65}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,9 +23,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,19 +38,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>ID</t>
+    <t>principle</t>
   </si>
   <si>
-    <t>Role</t>
+    <t>teacher</t>
   </si>
   <si>
-    <t>Principle</t>
+    <t>hr</t>
   </si>
   <si>
-    <t>Teacher</t>
+    <t>role</t>
   </si>
   <si>
-    <t>HR</t>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -83,11 +86,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -103,7 +109,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Chủ đề Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -399,44 +405,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB76FA65-5A3C-4B78-9737-CE8F2510D256}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="46.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C2" s="1" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO permission (role) VALUE ('",B2,"');")</f>
+        <v>INSERT INTO permission (role) VALUE ('principle');</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C3" s="1" t="str">
+        <f t="shared" ref="C3:C4" si="0">_xlfn.CONCAT("INSERT INTO permission (role) VALUE ('",B3,"');")</f>
+        <v>INSERT INTO permission (role) VALUE ('teacher');</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
+      <c r="C4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO permission (role) VALUE ('hr');</v>
       </c>
     </row>
   </sheetData>

</xml_diff>